<commit_message>
update input data table on search result for error log
</commit_message>
<xml_diff>
--- a/logsearch/data/error_logs/UC1_UC1_新人_03.xlsx
+++ b/logsearch/data/error_logs/UC1_UC1_新人_03.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\Desktop\work\logseach\ntt-backend\logsearch\data\error_logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ACA490-2B5C-4963-8ACB-734E923C4A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,63 +25,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pc_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">win_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">win_urlpath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">win_hwnd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">win_class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capimg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">explanation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">error_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">error_content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">window_open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ryoma Takahashi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DESKTOP-Q316RCS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShortCut - Tablacus Explorer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TablacusExplorer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D:\te240227\TE64.exe</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>pc_name</t>
+  </si>
+  <si>
+    <t>win_title</t>
+  </si>
+  <si>
+    <t>win_urlpath</t>
+  </si>
+  <si>
+    <t>win_hwnd</t>
+  </si>
+  <si>
+    <t>win_class</t>
+  </si>
+  <si>
+    <t>app_path</t>
+  </si>
+  <si>
+    <t>capimg</t>
+  </si>
+  <si>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t>error_type</t>
+  </si>
+  <si>
+    <t>error_content</t>
+  </si>
+  <si>
+    <t>window_open</t>
+  </si>
+  <si>
+    <t>Ryoma Takahashi</t>
+  </si>
+  <si>
+    <t>DESKTOP-Q316RCS</t>
+  </si>
+  <si>
+    <t>ShortCut - Tablacus Explorer</t>
+  </si>
+  <si>
+    <t>TablacusExplorer</t>
+  </si>
+  <si>
+    <t>D:\te240227\TE64.exe</t>
   </si>
   <si>
     <r>
@@ -87,7 +92,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">XX</t>
+      <t>XX</t>
     </r>
     <r>
       <rPr>
@@ -107,50 +112,47 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Google Chrome</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Chrome_WidgetWin_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Program Files\Google\Chrome\Application\chrome.exe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Book1.xlsx - Excel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D:\Work\Book1.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XLMAIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Program Files (x86)\Microsoft Office\Office16\EXCEL.EXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Users\Ryoma Takahashi\Desktop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Windows\explorer.exe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">operation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file:///D:/Work/AS%E7%A0%94/Git/Documents_BIST_Tsukuba2024/99_%E3%81%9D%E3%81%AE%E4%BB%96/20240415_%E6%A5%AD%E5%8B%99%E6%94%B9%E5%96%84%E3%83%87%E3%83%A2%E3%82%B7%E3%83%8A%E3%83%AA%E3%82%AA_%E8%8D%89%E6%A1%88/mainpage.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bdot20240415_141953/0415_141958_0.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">「商品納入・工事予約管理システム」を押下する</t>
+      <t>- Google Chrome</t>
+    </r>
+  </si>
+  <si>
+    <t>Chrome_WidgetWin_1</t>
+  </si>
+  <si>
+    <t>C:\Program Files\Google\Chrome\Application\chrome.exe</t>
+  </si>
+  <si>
+    <t>Book1.xlsx - Excel</t>
+  </si>
+  <si>
+    <t>D:\Work\Book1.xlsx</t>
+  </si>
+  <si>
+    <t>XLMAIN</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\Microsoft Office\Office16\EXCEL.EXE</t>
+  </si>
+  <si>
+    <t>Program Manager</t>
+  </si>
+  <si>
+    <t>C:\Users\Ryoma Takahashi\Desktop</t>
+  </si>
+  <si>
+    <t>Progman</t>
+  </si>
+  <si>
+    <t>C:\Windows\explorer.exe</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>file:///D:/Work/AS%E7%A0%94/Git/Documents_BIST_Tsukuba2024/99_%E3%81%9D%E3%81%AE%E4%BB%96/20240415_%E6%A5%AD%E5%8B%99%E6%94%B9%E5%96%84%E3%83%87%E3%83%A2%E3%82%B7%E3%83%8A%E3%83%AA%E3%82%AA_%E8%8D%89%E6%A1%88/mainpage.html</t>
+  </si>
+  <si>
+    <t>「商品納入・工事予約管理システム」を押下する</t>
   </si>
   <si>
     <r>
@@ -191,14 +193,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">- Google Chrome</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">file:///D:/Work/AS%E7%A0%94/Git/Documents_BIST_Tsukuba2024/99_%E3%81%9D%E3%81%AE%E4%BB%96/20240415_%E6%A5%AD%E5%8B%99%E6%94%B9%E5%96%84%E3%83%87%E3%83%A2%E3%82%B7%E3%83%8A%E3%83%AA%E3%82%AA_%E8%8D%89%E6%A1%88/reserve/loginpage_reserve.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bdot20240415_141953/0415_142001_0.png</t>
+      <t>- Google Chrome</t>
+    </r>
+  </si>
+  <si>
+    <t>file:///D:/Work/AS%E7%A0%94/Git/Documents_BIST_Tsukuba2024/99_%E3%81%9D%E3%81%AE%E4%BB%96/20240415_%E6%A5%AD%E5%8B%99%E6%94%B9%E5%96%84%E3%83%87%E3%83%A2%E3%82%B7%E3%83%8A%E3%83%AA%E3%82%AA_%E8%8D%89%E6%A1%88/reserve/loginpage_reserve.html</t>
   </si>
   <si>
     <r>
@@ -209,7 +208,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">「予約管理システム」へ「</t>
+      <t>「予約管理システム」へ「</t>
     </r>
     <r>
       <rPr>
@@ -219,7 +218,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">shinnjin</t>
+      <t>shinnjin</t>
     </r>
     <r>
       <rPr>
@@ -229,11 +228,11 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">」を入力する</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">error</t>
+      <t>」を入力する</t>
+    </r>
+  </si>
+  <si>
+    <t>error</t>
   </si>
   <si>
     <r>
@@ -254,7 +253,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">A</t>
+      <t>A</t>
     </r>
   </si>
   <si>
@@ -266,7 +265,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">ユーザー名「</t>
+      <t>ユーザー名「</t>
     </r>
     <r>
       <rPr>
@@ -276,7 +275,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">shinnjin</t>
+      <t>shinnjin</t>
     </r>
     <r>
       <rPr>
@@ -286,7 +285,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">」は無効です。</t>
+      <t>」は無効です。</t>
     </r>
   </si>
   <si>
@@ -298,7 +297,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">「予約管理システム」へ「</t>
+      <t>「予約管理システム」へ「</t>
     </r>
     <r>
       <rPr>
@@ -308,7 +307,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">shinjin</t>
+      <t>shinjin</t>
     </r>
     <r>
       <rPr>
@@ -318,7 +317,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">」を入力する</t>
+      <t>」を入力する</t>
     </r>
   </si>
   <si>
@@ -330,7 +329,7 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">「予約管理システム」へ「</t>
+      <t>「予約管理システム」へ「</t>
     </r>
     <r>
       <rPr>
@@ -340,7 +339,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">&lt;PASSWORD&gt;</t>
+      <t>&lt;PASSWORD&gt;</t>
     </r>
     <r>
       <rPr>
@@ -350,23 +349,74 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t xml:space="preserve">」を入力する</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">「送信」を押下する</t>
+      <t>」を入力する</t>
+    </r>
+  </si>
+  <si>
+    <t>「送信」を押下する</t>
+  </si>
+  <si>
+    <r>
+      <t>UC1/UC1_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>新人</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>/bdot20240415_141953/0415_141958_0.png</t>
+    </r>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <r>
+      <t>UC1/UC1_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>新人</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>/bdot20240415_141953/0415_142001_0.png</t>
+    </r>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ h:mm"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy\ h:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd\ h:mm"/>
+    <numFmt numFmtId="177" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -375,25 +425,7 @@
       <charset val="128"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -415,7 +447,7 @@
       <charset val="128"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF467886"/>
       <name val="Arial"/>
@@ -423,9 +455,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF467886"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -440,7 +478,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -448,77 +486,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -577,42 +564,350 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.41015625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="50.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="44.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="30.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="45.6"/>
+    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="19.25" customWidth="1"/>
+    <col min="4" max="4" width="18.25" customWidth="1"/>
+    <col min="5" max="5" width="35.25" customWidth="1"/>
+    <col min="6" max="6" width="21.375" customWidth="1"/>
+    <col min="7" max="7" width="9.75" customWidth="1"/>
+    <col min="8" max="8" width="19.125" customWidth="1"/>
+    <col min="9" max="9" width="50.25" customWidth="1"/>
+    <col min="10" max="10" width="37" customWidth="1"/>
+    <col min="11" max="11" width="44.75" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="30.25" customWidth="1"/>
+    <col min="29" max="29" width="20.625" customWidth="1"/>
+    <col min="31" max="31" width="45.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -670,9 +965,9 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>45398.5971527778</v>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A2" s="4">
+        <v>45398.597152777802</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
@@ -686,7 +981,7 @@
       <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>66644</v>
       </c>
       <c r="H2" s="5" t="s">
@@ -696,9 +991,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>45398.5971527778</v>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A3" s="4">
+        <v>45398.597152777802</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>13</v>
@@ -712,7 +1007,7 @@
       <c r="E3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3">
         <v>197686</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -722,9 +1017,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>45398.5971527778</v>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A4" s="4">
+        <v>45398.597152777802</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>13</v>
@@ -741,7 +1036,7 @@
       <c r="F4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4">
         <v>657346</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -751,9 +1046,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>45398.5971527778</v>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A5" s="4">
+        <v>45398.597152777802</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
@@ -770,7 +1065,7 @@
       <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5">
         <v>65824</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -780,9 +1075,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>45398.5971990741</v>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A6" s="4">
+        <v>45398.597199074102</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>30</v>
@@ -799,7 +1094,7 @@
       <c r="F6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>197686</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -809,15 +1104,15 @@
         <v>21</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>45398.5972337963</v>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A7" s="4">
+        <v>45398.597233796303</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>30</v>
@@ -828,13 +1123,13 @@
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>197686</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -844,18 +1139,18 @@
         <v>21</v>
       </c>
       <c r="J7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A8" s="4">
+        <v>45398.597233796303</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>45398.5972337963</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>14</v>
@@ -863,13 +1158,13 @@
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8">
         <v>197686</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -878,16 +1173,22 @@
       <c r="I8" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="J8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
       <c r="L8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>45398.5972337963</v>
+        <v>37</v>
+      </c>
+      <c r="M8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A9" s="4">
+        <v>45398.597233796303</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>30</v>
@@ -898,13 +1199,13 @@
       <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9">
         <v>197686</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -914,15 +1215,15 @@
         <v>21</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>45398.5972685185</v>
+        <v>43</v>
+      </c>
+      <c r="K9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A10" s="4">
+        <v>45398.597268518497</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>30</v>
@@ -933,13 +1234,13 @@
       <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10">
         <v>197686</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -949,15 +1250,15 @@
         <v>21</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
-        <v>45398.5972685185</v>
+        <v>43</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="A11" s="4">
+        <v>45398.597268518497</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>30</v>
@@ -968,13 +1269,13 @@
       <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11">
         <v>197686</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -984,65 +1285,61 @@
         <v>21</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="0" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A14" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="4"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A38" s="4"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <phoneticPr fontId="6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>